<commit_message>
prototype and today's work
</commit_message>
<xml_diff>
--- a/Work sheet.xlsx
+++ b/Work sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAMESH\Desktop\Quizgator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B489DB0C-C804-4E85-AC19-6BDA605349FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B97EB5-9057-40D4-985E-5A0A9249BD95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Table 1</t>
   </si>
@@ -53,6 +53,31 @@
   </si>
   <si>
     <t xml:space="preserve">search about firebase and how it's feature works. </t>
+  </si>
+  <si>
+    <t>date:11/1/2019</t>
+  </si>
+  <si>
+    <t>Research about technologies which are required for following!
+ 1. front-end:Xml,html,css
+ 2. back-end:java,php,python,
+ 3. server:aws,Apache,Firebase
+ 4. database:MongoDB,SQLite,Mysql,Firebase(Real time database) etc..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search about technology required for front-end,bach-end,server,database of application </t>
+  </si>
+  <si>
+    <t>search abiut the formate of quiz</t>
+  </si>
+  <si>
+    <t>https://www.quiz-zone.co.uk/runningaquiz/format.html</t>
+  </si>
+  <si>
+    <t>https://cdl.ucf.edu/support/webcourses/respondus/quiz-formatting-guidelines/</t>
+  </si>
+  <si>
+    <t>prototype of quiz app in adob xd</t>
   </si>
 </sst>
 </file>
@@ -225,7 +250,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -250,9 +275,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -264,6 +286,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1432,26 +1463,26 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
     <col min="5" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.6" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1480,10 +1511,10 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>0.4861111111111111</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1492,27 +1523,47 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:7" ht="98.25" customHeight="1">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:7" ht="26.25" customHeight="1">
       <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="13">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">

</xml_diff>

<commit_message>
Material theme XD resources
</commit_message>
<xml_diff>
--- a/Work sheet.xlsx
+++ b/Work sheet.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Table 1</t>
   </si>
@@ -22,6 +20,9 @@
     <t>Serial number</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Start time</t>
   </si>
   <si>
@@ -46,15 +47,23 @@
     <t>8:30pm</t>
   </si>
   <si>
-    <t>www.webquiz.it,www.pewinternet.org</t>
-  </si>
-  <si>
     <t>*create model of web and design home,login,profile,register pages and create form for adding quiz by admin.*know more about firebase database and how to use.</t>
   </si>
   <si>
     <t>see some quiz web how it work and in which effective manner quiz is display.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>www.webquiz.it,www.pewinternet.org</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">7:00pm </t>
   </si>
   <si>
@@ -64,20 +73,31 @@
     <t>*create protoype using addobe xd rethink about databases and use mongodb database for web.</t>
   </si>
   <si>
-    <t>https://www.quora.com/Which-is-better-MongoDB-or-Firebase</t>
+    <t>easy to connect codigniter with mongodb then firebase and provide some useful  fiture then firebase</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="15"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.quora.com/Which-is-better-MongoDB-or-Firebase</t>
+    </r>
   </si>
   <si>
     <t>To create web for *front-end:codigniter framework,jquery,ajax*backend:firebase and mongoDB  *server:wamp</t>
-  </si>
-  <si>
-    <t>easy to connect codigniter with mongodb then firebase and provide some useful  fiture then firebase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -89,19 +109,24 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color indexed="15"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +145,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -133,6 +164,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -146,7 +199,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -155,7 +208,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -164,43 +217,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -209,162 +262,171 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+  </cellStyleXfs>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFBDC0BF"/>
-      <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF3F3F3F"/>
-      <rgbColor rgb="FFDBDBDB"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -374,10 +436,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -554,40 +616,43 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -612,7 +677,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -638,7 +703,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +729,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -690,7 +755,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -716,7 +781,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -742,7 +807,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -768,7 +833,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -794,7 +859,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,7 +885,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -833,15 +898,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -850,15 +909,15 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -877,7 +936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +1040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +1066,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1092,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1118,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1144,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1111,7 +1170,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1124,15 +1183,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1146,26 +1199,26 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1195,7 +1248,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1221,7 +1274,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1247,7 +1300,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1273,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1299,7 +1352,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1378,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1351,7 +1404,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1377,7 +1430,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,7 +1456,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1416,301 +1469,315 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="256" width="16.36328125" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.65" customHeight="1">
-      <c r="A1" s="10" t="s">
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" ht="32.25" customHeight="1">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="125.5" customHeight="1">
-      <c r="A3" s="3">
+      <c r="H2" t="s" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="125.5" customHeight="1">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="10">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="94.5" customHeight="1">
-      <c r="A4" s="6">
+      <c r="G3" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" ht="94.5" customHeight="1">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s" s="15">
         <v>15</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" t="s" s="15">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s" s="15">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="20" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="20" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="20" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="H4" t="s" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" ht="20" customHeight="1">
+      <c r="A12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" s="16"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" ht="20" customHeight="1">
+      <c r="A15" s="16"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" ht="20" customHeight="1">
+      <c r="A16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" ht="20" customHeight="1">
+      <c r="A18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" ht="20" customHeight="1">
+      <c r="A19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" s="16"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" s="16"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="G4" r:id="rId2" location="" tooltip="" display=""/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>